<commit_message>
Final data update for PR
</commit_message>
<xml_diff>
--- a/Fitness.xlsx
+++ b/Fitness.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataScientistAccompli\projets\divertissements\fitness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE8171A-A708-4309-99E3-BC4E8CCF30C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12731532-292D-4F77-BDF3-AB2BF649F571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{C3DC8947-8663-41C9-9248-123E05F6B9AA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="292">
   <si>
     <t>Jour 1</t>
   </si>
@@ -841,6 +841,69 @@
   </si>
   <si>
     <t>18h47</t>
+  </si>
+  <si>
+    <t>17h31</t>
+  </si>
+  <si>
+    <t>16h08</t>
+  </si>
+  <si>
+    <t>21h07</t>
+  </si>
+  <si>
+    <t>18h26</t>
+  </si>
+  <si>
+    <t>19h04</t>
+  </si>
+  <si>
+    <t>8h15</t>
+  </si>
+  <si>
+    <t>7h40</t>
+  </si>
+  <si>
+    <t>20h42</t>
+  </si>
+  <si>
+    <t>21h52</t>
+  </si>
+  <si>
+    <t>9h36</t>
+  </si>
+  <si>
+    <t>7h09</t>
+  </si>
+  <si>
+    <t>11h36</t>
+  </si>
+  <si>
+    <t>10h58</t>
+  </si>
+  <si>
+    <t>22h00</t>
+  </si>
+  <si>
+    <t>7h14</t>
+  </si>
+  <si>
+    <t>21h13</t>
+  </si>
+  <si>
+    <t>23h11</t>
+  </si>
+  <si>
+    <t>17h30</t>
+  </si>
+  <si>
+    <t>6h40</t>
+  </si>
+  <si>
+    <t>9h22</t>
+  </si>
+  <si>
+    <t>20h44</t>
   </si>
 </sst>
 </file>
@@ -1236,10 +1299,10 @@
   <dimension ref="A1:BU11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AT13" sqref="AT13"/>
+      <selection pane="bottomRight" activeCell="BJ18" sqref="BJ18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1599,6 +1662,48 @@
       <c r="BE2" t="s">
         <v>269</v>
       </c>
+      <c r="BF2" t="s">
+        <v>271</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>272</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>274</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>276</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>280</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>281</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>282</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>283</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>285</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>248</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>288</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>274</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>289</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>290</v>
+      </c>
       <c r="BT2">
         <v>1</v>
       </c>
@@ -1703,6 +1808,21 @@
       <c r="BE3" t="s">
         <v>270</v>
       </c>
+      <c r="BG3" t="s">
+        <v>273</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>275</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>278</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>286</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>291</v>
+      </c>
       <c r="BT3">
         <v>1</v>
       </c>
@@ -1851,6 +1971,21 @@
       <c r="AD5" t="s">
         <v>202</v>
       </c>
+      <c r="BF5" t="s">
+        <v>112</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>253</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>107</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>284</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>135</v>
+      </c>
       <c r="BT5">
         <v>1</v>
       </c>
@@ -1942,6 +2077,15 @@
       <c r="BD7" t="s">
         <v>268</v>
       </c>
+      <c r="BI7" t="s">
+        <v>279</v>
+      </c>
+      <c r="BN7" t="s">
+        <v>287</v>
+      </c>
+      <c r="BO7" t="s">
+        <v>135</v>
+      </c>
       <c r="BT7">
         <v>1</v>
       </c>
@@ -1992,6 +2136,9 @@
       <c r="BA8" t="s">
         <v>258</v>
       </c>
+      <c r="BI8" t="s">
+        <v>277</v>
+      </c>
       <c r="BT8">
         <v>0</v>
       </c>
@@ -2053,6 +2200,12 @@
       </c>
       <c r="BC9" t="s">
         <v>265</v>
+      </c>
+      <c r="BF9" t="s">
+        <v>141</v>
+      </c>
+      <c r="BN9" t="s">
+        <v>148</v>
       </c>
       <c r="BT9">
         <v>0</v>
@@ -2259,11 +2412,11 @@
       </c>
       <c r="J4">
         <f>7-COUNTBLANK(Suivi!BF2:BL2)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K4">
         <f>7-COUNTBLANK(Suivi!BM2:BS2)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -2304,11 +2457,11 @@
       </c>
       <c r="J5">
         <f>7-COUNTBLANK(Suivi!BF3:BL3)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K5">
         <f>7-COUNTBLANK(Suivi!BM3:BS3)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -2394,7 +2547,7 @@
       </c>
       <c r="J7">
         <f>7-COUNTBLANK(Suivi!BF5:BL5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K7">
         <f>7-COUNTBLANK(Suivi!BM5:BS5)</f>
@@ -2484,11 +2637,11 @@
       </c>
       <c r="J9">
         <f>7-COUNTBLANK(Suivi!BF7:BL7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <f>7-COUNTBLANK(Suivi!BM7:BS7)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -2529,7 +2682,7 @@
       </c>
       <c r="J10">
         <f>7-COUNTBLANK(Suivi!BF8:BL8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <f>7-COUNTBLANK(Suivi!BM8:BS8)</f>
@@ -2574,11 +2727,11 @@
       </c>
       <c r="J11">
         <f>7-COUNTBLANK(Suivi!BF9:BL9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <f>7-COUNTBLANK(Suivi!BM9:BS9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -2752,11 +2905,11 @@
       </c>
       <c r="K21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -2800,11 +2953,11 @@
       </c>
       <c r="K22">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>42.857142857142854</v>
       </c>
       <c r="L22">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28.571428571428569</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
@@ -2896,7 +3049,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>83.333333333333343</v>
       </c>
       <c r="L24">
         <f t="shared" si="4"/>
@@ -2992,11 +3145,11 @@
       </c>
       <c r="K26">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L26">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
@@ -3040,7 +3193,7 @@
       </c>
       <c r="K27">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L27">
         <f t="shared" si="7"/>
@@ -3088,11 +3241,11 @@
       </c>
       <c r="K28">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L28">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
@@ -3339,11 +3492,11 @@
       </c>
       <c r="J5">
         <f>RANK('Point Hebdomadaire'!J5,'Point Hebdomadaire'!J$4:J$13)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K5">
         <f>RANK('Point Hebdomadaire'!K5,'Point Hebdomadaire'!K$4:K$13)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -3384,11 +3537,11 @@
       </c>
       <c r="J6">
         <f>RANK('Point Hebdomadaire'!J6,'Point Hebdomadaire'!J$4:J$13)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K6">
         <f>RANK('Point Hebdomadaire'!K6,'Point Hebdomadaire'!K$4:K$13)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -3429,11 +3582,11 @@
       </c>
       <c r="J7">
         <f>RANK('Point Hebdomadaire'!J7,'Point Hebdomadaire'!J$4:J$13)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K7">
         <f>RANK('Point Hebdomadaire'!K7,'Point Hebdomadaire'!K$4:K$13)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -3474,11 +3627,11 @@
       </c>
       <c r="J8">
         <f>RANK('Point Hebdomadaire'!J8,'Point Hebdomadaire'!J$4:J$13)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K8">
         <f>RANK('Point Hebdomadaire'!K8,'Point Hebdomadaire'!K$4:K$13)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -3519,11 +3672,11 @@
       </c>
       <c r="J9">
         <f>RANK('Point Hebdomadaire'!J9,'Point Hebdomadaire'!J$4:J$13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K9">
         <f>RANK('Point Hebdomadaire'!K9,'Point Hebdomadaire'!K$4:K$13)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -3564,11 +3717,11 @@
       </c>
       <c r="J10">
         <f>RANK('Point Hebdomadaire'!J10,'Point Hebdomadaire'!J$4:J$13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K10">
         <f>RANK('Point Hebdomadaire'!K10,'Point Hebdomadaire'!K$4:K$13)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -3609,11 +3762,11 @@
       </c>
       <c r="J11">
         <f>RANK('Point Hebdomadaire'!J11,'Point Hebdomadaire'!J$4:J$13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K11">
         <f>RANK('Point Hebdomadaire'!K11,'Point Hebdomadaire'!K$4:K$13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -3654,11 +3807,11 @@
       </c>
       <c r="J12">
         <f>RANK('Point Hebdomadaire'!J12,'Point Hebdomadaire'!J$4:J$13)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K12">
         <f>RANK('Point Hebdomadaire'!K12,'Point Hebdomadaire'!K$4:K$13)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -3699,11 +3852,11 @@
       </c>
       <c r="J13">
         <f>RANK('Point Hebdomadaire'!J13,'Point Hebdomadaire'!J$4:J$13)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K13">
         <f>RANK('Point Hebdomadaire'!K13,'Point Hebdomadaire'!K$4:K$13)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -3826,11 +3979,11 @@
       </c>
       <c r="J28">
         <f>RANK('Point Hebdomadaire'!K22,'Point Hebdomadaire'!K$21:K$29)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K28">
         <f>RANK('Point Hebdomadaire'!L22,'Point Hebdomadaire'!L$21:L$29)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -3871,11 +4024,11 @@
       </c>
       <c r="J29">
         <f>RANK('Point Hebdomadaire'!K23,'Point Hebdomadaire'!K$21:K$29)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K29">
         <f>RANK('Point Hebdomadaire'!L23,'Point Hebdomadaire'!L$21:L$29)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -3916,11 +4069,11 @@
       </c>
       <c r="J30">
         <f>RANK('Point Hebdomadaire'!K24,'Point Hebdomadaire'!K$21:K$29)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K30">
         <f>RANK('Point Hebdomadaire'!L24,'Point Hebdomadaire'!L$21:L$29)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -3961,11 +4114,11 @@
       </c>
       <c r="J31">
         <f>RANK('Point Hebdomadaire'!K25,'Point Hebdomadaire'!K$21:K$29)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K31">
         <f>RANK('Point Hebdomadaire'!L25,'Point Hebdomadaire'!L$21:L$29)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -4006,11 +4159,11 @@
       </c>
       <c r="J32">
         <f>RANK('Point Hebdomadaire'!K26,'Point Hebdomadaire'!K$21:K$29)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K32">
         <f>RANK('Point Hebdomadaire'!L26,'Point Hebdomadaire'!L$21:L$29)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -4051,11 +4204,11 @@
       </c>
       <c r="J33">
         <f>RANK('Point Hebdomadaire'!K27,'Point Hebdomadaire'!K$21:K$29)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K33">
         <f>RANK('Point Hebdomadaire'!L27,'Point Hebdomadaire'!L$21:L$29)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
@@ -4096,11 +4249,11 @@
       </c>
       <c r="J34">
         <f>RANK('Point Hebdomadaire'!K28,'Point Hebdomadaire'!K$21:K$29)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K34">
         <f>RANK('Point Hebdomadaire'!L28,'Point Hebdomadaire'!L$21:L$29)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -4141,11 +4294,11 @@
       </c>
       <c r="J35">
         <f>RANK('Point Hebdomadaire'!K29,'Point Hebdomadaire'!K$21:K$29)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K35">
         <f>RANK('Point Hebdomadaire'!L29,'Point Hebdomadaire'!L$21:L$29)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>